<commit_message>
Added Sushant's Belbin's Analysis and updated Team Belbin's Analysis
</commit_message>
<xml_diff>
--- a/Project Planning/Skills Audit/Individual Skill Audit/Kadamber Verma.xlsx
+++ b/Project Planning/Skills Audit/Individual Skill Audit/Kadamber Verma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\L5\Semester-2\MANA541 - Project Management - 14805 - WIN - 201910\The-Clehuderfax-e-chain\Project Planning\Skills Audit\Individual Skill Audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74459DE-11D9-411B-9752-D340F160A71C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CE8566-12E4-4575-8191-19CE504D0517}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="23640" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1088,8 +1088,8 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1202,7 +1202,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>46</v>
@@ -1256,7 +1256,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>48</v>
@@ -1310,7 +1310,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>49</v>
@@ -1319,7 +1319,7 @@
         <v>29</v>
       </c>
       <c r="F11" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="9">
         <v>43891</v>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>6</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>50</v>
@@ -1346,7 +1346,7 @@
         <v>31</v>
       </c>
       <c r="F12" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="9">
         <v>43893</v>
@@ -1364,7 +1364,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>49</v>
@@ -1373,7 +1373,7 @@
         <v>30</v>
       </c>
       <c r="F13" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="9">
         <v>43896</v>
@@ -1418,7 +1418,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>45</v>
@@ -1445,7 +1445,7 @@
         <v>21</v>
       </c>
       <c r="C16" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>44</v>
@@ -1472,7 +1472,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>43</v>
@@ -1498,7 +1498,7 @@
         <v>20</v>
       </c>
       <c r="C18" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>44</v>
@@ -1524,7 +1524,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>42</v>
@@ -1550,7 +1550,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>52</v>
@@ -1576,7 +1576,7 @@
         <v>35</v>
       </c>
       <c r="C21" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>50</v>
@@ -1585,7 +1585,7 @@
         <v>39</v>
       </c>
       <c r="F21" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="9">
         <v>43893</v>
@@ -1602,7 +1602,7 @@
         <v>37</v>
       </c>
       <c r="C22" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>53</v>
@@ -1611,7 +1611,7 @@
         <v>40</v>
       </c>
       <c r="F22" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" s="9">
         <v>43898</v>
@@ -1628,7 +1628,7 @@
         <v>36</v>
       </c>
       <c r="C23" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>50</v>

</xml_diff>